<commit_message>
Add send to email
</commit_message>
<xml_diff>
--- a/income&expenses.xlsx
+++ b/income&expenses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phanuruj Sotthidat\Documents\Fodder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiss\OneDrive\Documents\UiPath\Fodder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49857A3A-109C-45AC-BD12-40DEE52D8C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4CF4D4-5C20-43CF-BE49-3D22573FB923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -45,18 +45,6 @@
   </si>
   <si>
     <t>Outcome</t>
-  </si>
-  <si>
-    <t>SCB Easy</t>
-  </si>
-  <si>
-    <t>7-Eleven</t>
-  </si>
-  <si>
-    <t>The Sand Dollar</t>
-  </si>
-  <si>
-    <t>HARBOR LANE CAFE</t>
   </si>
 </sst>
 </file>
@@ -91,10 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,105 +412,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45050</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45050</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45049</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>45049</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>45048</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>45048</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>57242</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>43629</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>82.98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>43789</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1">
-        <v>31.39</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
final jing jing la
</commit_message>
<xml_diff>
--- a/income&expenses.xlsx
+++ b/income&expenses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiss\OneDrive\Documents\UiPath\Fodder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phanuruj Sotthidat\Documents\Fodder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4CF4D4-5C20-43CF-BE49-3D22573FB923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFC3D1C-1EA9-4BC9-8A8C-79D301A60AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Receipt" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>Outcome</t>
+  </si>
+  <si>
+    <t>SCB Easy</t>
+  </si>
+  <si>
+    <t>7-Eleven</t>
+  </si>
+  <si>
+    <t>The Sand Dollar</t>
+  </si>
+  <si>
+    <t>HARBOR LANE CAFE</t>
   </si>
 </sst>
 </file>
@@ -79,9 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +425,182 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45063</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45062</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45062</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>45059</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>340.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>320.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45055</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>57242</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43629</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>82.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43789</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1">
+        <v>31.39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>